<commit_message>
Load and copy images on worksheets.
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/ImageHandling/ImageAnchors.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/ImageHandling/ImageAnchors.xlsx
@@ -76,10 +76,10 @@
 </x:styleSheet>
 </file>
 
-<file path=xl/drawings/drawing.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:absoluteAnchor>
-    <xdr:pos x="2095792" y="1428949"/>
+    <xdr:pos x="2086266" y="1419423"/>
     <xdr:ext cx="2400635" cy="1448002"/>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -138,7 +138,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:twoCellAnchor>
     <xdr:from>

</xml_diff>

<commit_message>
First rework of Picture API
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/ImageHandling/ImageAnchors.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/ImageHandling/ImageAnchors.xlsx
@@ -89,7 +89,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="Image10" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="rId7" cstate="print"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -120,7 +120,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="Image11" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="rId8" cstate="print"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -161,7 +161,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="Image20" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="rId10" cstate="print"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -477,7 +477,7 @@
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
-  <x:drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Image10"/>
+  <x:drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
   <x:tableParts count="0"/>
 </x:worksheet>
 </file>
@@ -497,7 +497,7 @@
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
-  <x:drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Image20"/>
+  <x:drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
   <x:tableParts count="0"/>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
More image API improvements.
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/ImageHandling/ImageAnchors.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/ImageHandling/ImageAnchors.xlsx
@@ -77,29 +77,29 @@
 </file>
 
 <file path=xl/drawings/drawing.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:absoluteAnchor>
-    <xdr:pos x="2095792" y="1428949"/>
-    <xdr:ext cx="2400635" cy="1448002"/>
+    <xdr:pos x="2095500" y="1428750"/>
+    <xdr:ext cx="2400300" cy="1447800"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="1" name="Image10"/>
         <xdr:cNvPicPr>
-          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1" noMove="1" noResize="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="rId7" cstate="print"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:blip r:embed="rId7" cstate="print"/>
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2400635" cy="1448002"/>
+          <a:ext cx="2400300" cy="1447800"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+        <a:prstGeom prst="rect"/>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -111,26 +111,26 @@
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="2400635" cy="1448002"/>
+    <xdr:ext cx="2400300" cy="1447800"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Image11"/>
         <xdr:cNvPicPr>
-          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1" noMove="1" noResize="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="rId8" cstate="print"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:blip r:embed="rId8" cstate="print"/>
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2400635" cy="1448002"/>
+          <a:ext cx="2400300" cy="1447800"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+        <a:prstGeom prst="rect"/>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -139,7 +139,7 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
@@ -157,21 +157,21 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="1" name="Image20"/>
         <xdr:cNvPicPr>
-          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1" noMove="1" noResize="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="rId10" cstate="print"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:blip r:embed="rId10" cstate="print"/>
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2400635" cy="1448002"/>
+          <a:ext cx="2400300" cy="1447800"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+        <a:prstGeom prst="rect"/>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -467,12 +467,17 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1"/>
+  <x:dimension ref="A1:A1"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
-  <x:sheetData/>
+  <x:cols>
+    <x:col min="1" max="1" width="9.140625" style="0" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="1:1"/>
+  </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
@@ -487,12 +492,18 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1"/>
+  <x:dimension ref="A1:G9"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
-  <x:sheetData/>
+  <x:cols>
+    <x:col min="1" max="7" width="9.140625" style="0" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="6" spans="1:7"/>
+    <x:row r="9" spans="1:7"/>
+  </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>

</xml_diff>